<commit_message>
Commit of working database setup scripts
</commit_message>
<xml_diff>
--- a/Project/Documentation/menu.xlsx
+++ b/Project/Documentation/menu.xlsx
@@ -24,28 +24,10 @@
     <t>Thai style Mango Sauce Deep Fried Tofu</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Small</t>
   </si>
   <si>
     <t>Large</t>
-  </si>
-  <si>
-    <t>Size</t>
   </si>
   <si>
     <t>Thai Style Deep Fried Chicken Wings (12 pcs)</t>
@@ -129,9 +111,6 @@
   </si>
   <si>
     <t>Crab Meat with Fish Maw Soup</t>
-  </si>
-  <si>
-    <t>Spicy</t>
   </si>
   <si>
     <t>Noodle Soup</t>
@@ -692,6 +671,27 @@
 Assorted Mushrooms with Eggplant
 Breaded Shrimps
 Thai Style Fried Rice</t>
+  </si>
+  <si>
+    <t>intMenuNumber</t>
+  </si>
+  <si>
+    <t>strCategory</t>
+  </si>
+  <si>
+    <t>strMenuItemName</t>
+  </si>
+  <si>
+    <t>txtDescription</t>
+  </si>
+  <si>
+    <t>dblPrice</t>
+  </si>
+  <si>
+    <t>strSize</t>
+  </si>
+  <si>
+    <t>blnSpicy</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1051,25 +1051,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>208</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>212</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>213</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>7.95</v>
@@ -1108,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>8.9499999999999993</v>
@@ -1122,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>5.95</v>
@@ -1136,7 +1136,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>8.9499999999999993</v>
@@ -1150,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>9.9499999999999993</v>
@@ -1164,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>11.95</v>
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>2.95</v>
@@ -1192,7 +1192,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>7.95</v>
@@ -1206,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <v>4.95</v>
@@ -1220,7 +1220,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E12">
         <v>6.95</v>
@@ -1237,7 +1237,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E13">
         <v>4.95</v>
@@ -1254,7 +1254,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <v>5.95</v>
@@ -1271,7 +1271,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <v>8.9499999999999993</v>
@@ -1285,10 +1285,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>6.95</v>
@@ -1305,10 +1305,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>6.95</v>
@@ -1325,10 +1325,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>16.95</v>
@@ -1336,87 +1336,87 @@
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>3.5</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E20">
         <v>9.9499999999999993</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E21">
         <v>3.5</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E22">
         <v>9.9499999999999993</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E23">
         <v>4.5</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1424,19 +1424,19 @@
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E24">
         <v>9.9499999999999993</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1444,81 +1444,81 @@
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E25">
         <v>3.5</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E26">
         <v>9.9499999999999993</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E27">
         <v>3.5</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E28">
         <v>9.9499999999999993</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B29">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E29">
         <v>9.9499999999999993</v>
@@ -1526,81 +1526,81 @@
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B30">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E30">
         <v>3.5</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E31">
         <v>8.9499999999999993</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E32">
         <v>4.95</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E33">
         <v>10.95</v>
       </c>
       <c r="F33" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E34">
         <v>7.95</v>
@@ -1611,13 +1611,13 @@
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E35">
         <v>7.95</v>
@@ -1628,13 +1628,13 @@
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E36">
         <v>7.95</v>
@@ -1645,13 +1645,13 @@
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B37">
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E37">
         <v>7.95</v>
@@ -1659,47 +1659,47 @@
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B38">
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E38">
         <v>12.95</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B39">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E39">
         <v>12.95</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E40">
         <v>14.95</v>
@@ -1707,13 +1707,13 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E41">
         <v>9.9499999999999993</v>
@@ -1721,13 +1721,13 @@
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E42">
         <v>13.95</v>
@@ -1735,13 +1735,13 @@
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E43">
         <v>8.9499999999999993</v>
@@ -1749,13 +1749,13 @@
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B44">
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E44">
         <v>8.9499999999999993</v>
@@ -1763,13 +1763,13 @@
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B45">
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E45">
         <v>8.9499999999999993</v>
@@ -1777,13 +1777,13 @@
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B46">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E46">
         <v>11.95</v>
@@ -1791,13 +1791,13 @@
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E47">
         <v>13.95</v>
@@ -1805,13 +1805,13 @@
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B48">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E48">
         <v>13.95</v>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B49">
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E49">
         <v>12.95</v>
@@ -1833,13 +1833,13 @@
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B50">
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E50">
         <v>8.9499999999999993</v>
@@ -1847,13 +1847,13 @@
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B51">
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E51">
         <v>13.95</v>
@@ -1861,13 +1861,13 @@
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E52">
         <v>11.95</v>
@@ -1875,13 +1875,13 @@
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B53">
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E53">
         <v>11.95</v>
@@ -1889,13 +1889,13 @@
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B54">
         <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E54">
         <v>11.95</v>
@@ -1903,13 +1903,13 @@
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E55">
         <v>8.9499999999999993</v>
@@ -1917,13 +1917,13 @@
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E56">
         <v>13.95</v>
@@ -1931,13 +1931,13 @@
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E57">
         <v>13.95</v>
@@ -1945,13 +1945,13 @@
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B58">
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E58">
         <v>13.95</v>
@@ -1959,13 +1959,13 @@
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B59">
         <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E59">
         <v>13.95</v>
@@ -1973,13 +1973,13 @@
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B60">
         <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E60">
         <v>13.95</v>
@@ -1987,13 +1987,13 @@
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B61">
         <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E61">
         <v>9.9499999999999993</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B62">
         <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E62">
         <v>11.95</v>
@@ -2015,13 +2015,13 @@
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B63">
         <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E63">
         <v>10.95</v>
@@ -2029,13 +2029,13 @@
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B64">
         <v>25</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E64">
         <v>11.95</v>
@@ -2043,13 +2043,13 @@
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B65">
         <v>26</v>
       </c>
       <c r="C65" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E65">
         <v>8.9499999999999993</v>
@@ -2057,13 +2057,13 @@
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B66">
         <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E66">
         <v>9.9499999999999993</v>
@@ -2071,13 +2071,13 @@
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E67">
         <v>9.9499999999999993</v>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E68">
         <v>11.95</v>
@@ -2099,13 +2099,13 @@
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E69">
         <v>9.9499999999999993</v>
@@ -2116,13 +2116,13 @@
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B70">
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E70">
         <v>11.95</v>
@@ -2133,13 +2133,13 @@
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B71">
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E71">
         <v>11.95</v>
@@ -2147,13 +2147,13 @@
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B72">
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E72">
         <v>11.95</v>
@@ -2161,13 +2161,13 @@
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B73">
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E73">
         <v>13.95</v>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B74">
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E74">
         <v>10.95</v>
@@ -2189,13 +2189,13 @@
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B75">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E75">
         <v>9.9499999999999993</v>
@@ -2206,13 +2206,13 @@
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B76">
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E76">
         <v>9.9499999999999993</v>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B77">
         <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E77">
         <v>9.9499999999999993</v>
@@ -2237,13 +2237,13 @@
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B78">
         <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E78">
         <v>9.9499999999999993</v>
@@ -2251,13 +2251,13 @@
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B79">
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E79">
         <v>8.9499999999999993</v>
@@ -2265,13 +2265,13 @@
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B80">
         <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E80">
         <v>8.9499999999999993</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B81">
         <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E81">
         <v>11.95</v>
@@ -2293,13 +2293,13 @@
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B82">
         <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E82">
         <v>12.95</v>
@@ -2307,13 +2307,13 @@
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B83">
         <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E83">
         <v>11.95</v>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E84">
         <v>1.2</v>
@@ -2335,13 +2335,13 @@
     </row>
     <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E85">
         <v>2</v>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E86">
         <v>2</v>
@@ -2363,13 +2363,13 @@
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E87">
         <v>13.95</v>
@@ -2377,13 +2377,13 @@
     </row>
     <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B88">
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E88">
         <v>13.95</v>
@@ -2391,13 +2391,13 @@
     </row>
     <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B89">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E89">
         <v>11.93</v>
@@ -2408,13 +2408,13 @@
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E90">
         <v>13.95</v>
@@ -2425,13 +2425,13 @@
     </row>
     <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B91">
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E91">
         <v>13.95</v>
@@ -2439,13 +2439,13 @@
     </row>
     <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B92">
         <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E92">
         <v>9.9499999999999993</v>
@@ -2453,13 +2453,13 @@
     </row>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B93">
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E93">
         <v>9.9499999999999993</v>
@@ -2467,13 +2467,13 @@
     </row>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B94">
         <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E94">
         <v>9.9499999999999993</v>
@@ -2481,13 +2481,13 @@
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B95">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E95">
         <v>9.9499999999999993</v>
@@ -2495,13 +2495,13 @@
     </row>
     <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B96">
         <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E96">
         <v>9.9499999999999993</v>
@@ -2509,13 +2509,13 @@
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B97">
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E97">
         <v>9.9499999999999993</v>
@@ -2523,13 +2523,13 @@
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B98">
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E98">
         <v>10.95</v>
@@ -2537,13 +2537,13 @@
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B99">
         <v>13</v>
       </c>
       <c r="C99" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E99">
         <v>8.9499999999999993</v>
@@ -2554,13 +2554,13 @@
     </row>
     <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B100">
         <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E100">
         <v>13.95</v>
@@ -2568,13 +2568,13 @@
     </row>
     <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B101">
         <v>15</v>
       </c>
       <c r="C101" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E101">
         <v>9.9499999999999993</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B102">
         <v>16</v>
       </c>
       <c r="C102" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E102">
         <v>9.9499999999999993</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B103">
         <v>17</v>
       </c>
       <c r="C103" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E103">
         <v>9.9499999999999993</v>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E104">
         <v>9.9499999999999993</v>
@@ -2627,13 +2627,13 @@
     </row>
     <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B105">
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E105">
         <v>9.9499999999999993</v>
@@ -2644,13 +2644,13 @@
     </row>
     <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B106">
         <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E106">
         <v>10.95</v>
@@ -2658,13 +2658,13 @@
     </row>
     <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B107">
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E107">
         <v>9.9499999999999993</v>
@@ -2672,13 +2672,13 @@
     </row>
     <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E108">
         <v>8.9499999999999993</v>
@@ -2689,13 +2689,13 @@
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B109">
         <v>6</v>
       </c>
       <c r="C109" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E109">
         <v>8.9499999999999993</v>
@@ -2703,13 +2703,13 @@
     </row>
     <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B110">
         <v>7</v>
       </c>
       <c r="C110" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E110">
         <v>9.9499999999999993</v>
@@ -2717,13 +2717,13 @@
     </row>
     <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B111">
         <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E111">
         <v>9.9499999999999993</v>
@@ -2731,13 +2731,13 @@
     </row>
     <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B112">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E112">
         <v>9.9499999999999993</v>
@@ -2748,13 +2748,13 @@
     </row>
     <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B113">
         <v>10</v>
       </c>
       <c r="C113" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E113">
         <v>9.9499999999999993</v>
@@ -2765,13 +2765,13 @@
     </row>
     <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B114">
         <v>11</v>
       </c>
       <c r="C114" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E114">
         <v>13.95</v>
@@ -2779,13 +2779,13 @@
     </row>
     <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E115">
         <v>8.9499999999999993</v>
@@ -2793,13 +2793,13 @@
     </row>
     <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B116">
         <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E116">
         <v>9.9499999999999993</v>
@@ -2807,13 +2807,13 @@
     </row>
     <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B117">
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E117">
         <v>9.9499999999999993</v>
@@ -2821,13 +2821,13 @@
     </row>
     <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B118">
         <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E118">
         <v>12.95</v>
@@ -2835,13 +2835,13 @@
     </row>
     <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B119">
         <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E119">
         <v>8.9499999999999993</v>
@@ -2849,13 +2849,13 @@
     </row>
     <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E120">
         <v>6.95</v>
@@ -2866,13 +2866,13 @@
     </row>
     <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B121">
         <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E121">
         <v>8.9499999999999993</v>
@@ -2883,13 +2883,13 @@
     </row>
     <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B122">
         <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E122">
         <v>9.9499999999999993</v>
@@ -2900,13 +2900,13 @@
     </row>
     <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B123">
         <v>9</v>
       </c>
       <c r="C123" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E123">
         <v>8.9499999999999993</v>
@@ -2914,13 +2914,13 @@
     </row>
     <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B124">
         <v>10</v>
       </c>
       <c r="C124" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E124">
         <v>11.95</v>
@@ -2928,13 +2928,13 @@
     </row>
     <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B125">
         <v>11</v>
       </c>
       <c r="C125" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E125">
         <v>13.95</v>
@@ -2942,16 +2942,16 @@
     </row>
     <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B126">
         <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D126" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E126">
         <v>7.95</v>
@@ -2962,13 +2962,13 @@
     </row>
     <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B127">
         <v>13</v>
       </c>
       <c r="C127" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E127">
         <v>9.9499999999999993</v>
@@ -2979,13 +2979,13 @@
     </row>
     <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B128">
         <v>14</v>
       </c>
       <c r="C128" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E128">
         <v>9.9499999999999993</v>
@@ -2996,13 +2996,13 @@
     </row>
     <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B129">
         <v>15</v>
       </c>
       <c r="C129" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E129">
         <v>9.9499999999999993</v>
@@ -3013,13 +3013,13 @@
     </row>
     <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B130">
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E130">
         <v>8.9499999999999993</v>
@@ -3027,13 +3027,13 @@
     </row>
     <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B131">
         <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E131">
         <v>10.95</v>
@@ -3041,13 +3041,13 @@
     </row>
     <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B132">
         <v>3</v>
       </c>
       <c r="C132" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E132">
         <v>8.9499999999999993</v>
@@ -3058,13 +3058,13 @@
     </row>
     <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B133">
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E133">
         <v>9.9499999999999993</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B134">
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E134">
         <v>8.9499999999999993</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B135">
         <v>6</v>
       </c>
       <c r="C135" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E135">
         <v>8.9499999999999993</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B136">
         <v>7</v>
       </c>
       <c r="C136" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E136">
         <v>8.9499999999999993</v>
@@ -3114,13 +3114,13 @@
     </row>
     <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E137">
         <v>8.9499999999999993</v>
@@ -3128,13 +3128,13 @@
     </row>
     <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B138">
         <v>9</v>
       </c>
       <c r="C138" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E138">
         <v>9.9499999999999993</v>
@@ -3145,13 +3145,13 @@
     </row>
     <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B139">
         <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E139">
         <v>8.9499999999999993</v>
@@ -3159,13 +3159,13 @@
     </row>
     <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B140">
         <v>11</v>
       </c>
       <c r="C140" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E140">
         <v>8.9499999999999993</v>
@@ -3176,13 +3176,13 @@
     </row>
     <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B141">
         <v>12</v>
       </c>
       <c r="C141" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E141">
         <v>8.9499999999999993</v>
@@ -3190,13 +3190,13 @@
     </row>
     <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B142">
         <v>13</v>
       </c>
       <c r="C142" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E142">
         <v>8.9499999999999993</v>
@@ -3204,13 +3204,13 @@
     </row>
     <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B143">
         <v>14</v>
       </c>
       <c r="C143" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E143">
         <v>8.9499999999999993</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B144">
         <v>15</v>
       </c>
       <c r="C144" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E144">
         <v>11.95</v>
@@ -3235,13 +3235,13 @@
     </row>
     <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B145">
         <v>16</v>
       </c>
       <c r="C145" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E145">
         <v>12.95</v>
@@ -3249,13 +3249,13 @@
     </row>
     <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B146">
         <v>17</v>
       </c>
       <c r="C146" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E146">
         <v>10.95</v>
@@ -3263,13 +3263,13 @@
     </row>
     <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B147">
         <v>18</v>
       </c>
       <c r="C147" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E147">
         <v>8.9499999999999993</v>
@@ -3277,13 +3277,13 @@
     </row>
     <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B148">
         <v>19</v>
       </c>
       <c r="C148" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E148">
         <v>8.9499999999999993</v>
@@ -3291,13 +3291,13 @@
     </row>
     <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B149">
         <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E149">
         <v>9.9499999999999993</v>
@@ -3305,13 +3305,13 @@
     </row>
     <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B150">
         <v>2</v>
       </c>
       <c r="C150" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E150">
         <v>9.9499999999999993</v>
@@ -3319,13 +3319,13 @@
     </row>
     <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B151">
         <v>3</v>
       </c>
       <c r="C151" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E151">
         <v>10.95</v>
@@ -3333,13 +3333,13 @@
     </row>
     <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B152">
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E152">
         <v>9.9499999999999993</v>
@@ -3350,13 +3350,13 @@
     </row>
     <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B153">
         <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E153">
         <v>12.95</v>
@@ -3367,13 +3367,13 @@
     </row>
     <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B154">
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E154">
         <v>11.95</v>
@@ -3381,13 +3381,13 @@
     </row>
     <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B155">
         <v>7</v>
       </c>
       <c r="C155" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E155">
         <v>10.95</v>
@@ -3398,13 +3398,13 @@
     </row>
     <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B156">
         <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E156">
         <v>8.9499999999999993</v>
@@ -3412,13 +3412,13 @@
     </row>
     <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B157">
         <v>9</v>
       </c>
       <c r="C157" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E157">
         <v>7.95</v>
@@ -3426,13 +3426,13 @@
     </row>
     <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B158">
         <v>10</v>
       </c>
       <c r="C158" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E158">
         <v>7.95</v>
@@ -3440,13 +3440,13 @@
     </row>
     <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B159">
         <v>11</v>
       </c>
       <c r="C159" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E159">
         <v>7.95</v>
@@ -3454,13 +3454,13 @@
     </row>
     <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B160">
         <v>12</v>
       </c>
       <c r="C160" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E160">
         <v>7.95</v>
@@ -3471,13 +3471,13 @@
     </row>
     <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B161">
         <v>13</v>
       </c>
       <c r="C161" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E161">
         <v>12.95</v>
@@ -3485,13 +3485,13 @@
     </row>
     <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B162">
         <v>14</v>
       </c>
       <c r="C162" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E162">
         <v>10.95</v>
@@ -3499,13 +3499,13 @@
     </row>
     <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B163" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C163" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E163">
         <v>9.9499999999999993</v>
@@ -3513,13 +3513,13 @@
     </row>
     <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B164" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C164" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E164">
         <v>9.9499999999999993</v>
@@ -3527,13 +3527,13 @@
     </row>
     <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B165" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C165" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E165">
         <v>9.9499999999999993</v>
@@ -3544,13 +3544,13 @@
     </row>
     <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B166" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C166" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E166">
         <v>9.9499999999999993</v>
@@ -3558,13 +3558,13 @@
     </row>
     <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B167" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C167" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E167">
         <v>9.9499999999999993</v>
@@ -3572,13 +3572,13 @@
     </row>
     <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B168" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C168" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E168">
         <v>9.9499999999999993</v>
@@ -3586,13 +3586,13 @@
     </row>
     <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B169" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C169" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E169">
         <v>9.9499999999999993</v>
@@ -3600,13 +3600,13 @@
     </row>
     <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B170" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C170" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E170">
         <v>9.9499999999999993</v>
@@ -3614,13 +3614,13 @@
     </row>
     <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B171" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C171" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E171">
         <v>9.9499999999999993</v>
@@ -3631,13 +3631,13 @@
     </row>
     <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B172" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C172" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E172">
         <v>9.9499999999999993</v>
@@ -3645,13 +3645,13 @@
     </row>
     <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B173" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C173" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E173">
         <v>9.9499999999999993</v>
@@ -3659,13 +3659,13 @@
     </row>
     <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>186</v>
+      </c>
+      <c r="B174" t="s">
+        <v>181</v>
+      </c>
+      <c r="C174" t="s">
         <v>193</v>
-      </c>
-      <c r="B174" t="s">
-        <v>188</v>
-      </c>
-      <c r="C174" t="s">
-        <v>200</v>
       </c>
       <c r="E174">
         <v>9.9499999999999993</v>
@@ -3673,13 +3673,13 @@
     </row>
     <row r="175" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B175" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C175" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E175">
         <v>9.9499999999999993</v>
@@ -3690,13 +3690,13 @@
     </row>
     <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B176" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C176" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E176">
         <v>9.9499999999999993</v>
@@ -3707,13 +3707,13 @@
     </row>
     <row r="177" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B177" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C177" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E177">
         <v>9.9499999999999993</v>
@@ -3724,16 +3724,16 @@
     </row>
     <row r="178" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B178" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C178" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E178">
         <v>9.9499999999999993</v>
@@ -3741,16 +3741,16 @@
     </row>
     <row r="179" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B179">
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E179">
         <v>23.95</v>
@@ -3758,16 +3758,16 @@
     </row>
     <row r="180" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B180">
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E180">
         <v>30.95</v>
@@ -3775,16 +3775,16 @@
     </row>
     <row r="181" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B181">
         <v>3</v>
       </c>
       <c r="C181" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E181">
         <v>49.95</v>
@@ -3792,16 +3792,16 @@
     </row>
     <row r="182" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B182">
         <v>4</v>
       </c>
       <c r="C182" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E182">
         <v>63.95</v>
@@ -3809,16 +3809,16 @@
     </row>
     <row r="183" spans="1:7" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B183">
         <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E183">
         <v>77.95</v>

</xml_diff>